<commit_message>
added all test cases
</commit_message>
<xml_diff>
--- a/target/test-classes/capstonedata.xlsx
+++ b/target/test-classes/capstonedata.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geeth\OneDrive\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12494C34-A565-441E-A4E0-9B8444F5C125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCC6E01-4C64-4190-AD8F-436A40A0DDD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2FCBC044-FFB4-4B58-ACA2-C1DBAF96CC27}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{2FCBC044-FFB4-4B58-ACA2-C1DBAF96CC27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>firstname</t>
   </si>
@@ -52,19 +51,16 @@
     <t>confirm password</t>
   </si>
   <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>liki</t>
-  </si>
-  <si>
-    <t>saiiiii</t>
-  </si>
-  <si>
-    <t>likiiii456@gmail.com</t>
-  </si>
-  <si>
-    <t>liki@789</t>
+    <t>bkjh</t>
+  </si>
+  <si>
+    <t>jbkjhkj</t>
+  </si>
+  <si>
+    <t>ghjhkhkjhkhjhj56@gmail.com</t>
+  </si>
+  <si>
+    <t>bghjgkj@123</t>
   </si>
 </sst>
 </file>
@@ -446,7 +442,7 @@
   <cols>
     <col min="1" max="1" width="12.44140625" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -470,19 +466,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -493,22 +489,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2DC937-AD11-4078-BC34-8CC93C35BC43}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added all final test cases
</commit_message>
<xml_diff>
--- a/target/test-classes/capstonedata.xlsx
+++ b/target/test-classes/capstonedata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geeth\OneDrive\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02EEA3C-B7D9-402C-9F48-386B4B365047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B843C84-D28F-4DE7-8FD9-69770E3F19BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{2FCBC044-FFB4-4B58-ACA2-C1DBAF96CC27}"/>
   </bookViews>
@@ -51,16 +51,16 @@
     <t>confirm password</t>
   </si>
   <si>
-    <t>keerthiiiii</t>
-  </si>
-  <si>
-    <t>keeruuuuuu</t>
-  </si>
-  <si>
-    <t>keeruuuuu897@gmail.com</t>
-  </si>
-  <si>
-    <t>keeruuuuu@976</t>
+    <t>Keeru</t>
+  </si>
+  <si>
+    <t>keerthi</t>
+  </si>
+  <si>
+    <t>keerthi232@gmail.com</t>
+  </si>
+  <si>
+    <t>keerthi@232</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
     <col min="3" max="3" width="27.88671875" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -492,7 +492,7 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{1034C003-7280-4B81-BFE7-7B0FCC9FF90F}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{ED4BBD5B-FF58-44D2-AFA0-D39151440B74}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{943A62CF-578B-4607-BCC1-DB29C82756CA}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{18276693-60BD-4F59-B748-C03EB708A17E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
renamed xml file and did some modifications in code
</commit_message>
<xml_diff>
--- a/target/test-classes/capstonedata.xlsx
+++ b/target/test-classes/capstonedata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geeth\OneDrive\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B843C84-D28F-4DE7-8FD9-69770E3F19BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF8D532-D87E-4EAE-B27C-D0FF94AE9842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{2FCBC044-FFB4-4B58-ACA2-C1DBAF96CC27}"/>
   </bookViews>
@@ -57,10 +57,10 @@
     <t>keerthi</t>
   </si>
   <si>
-    <t>keerthi232@gmail.com</t>
-  </si>
-  <si>
-    <t>keerthi@232</t>
+    <t>keerthi2321@gmail.com</t>
+  </si>
+  <si>
+    <t>keerthi@2321</t>
   </si>
 </sst>
 </file>

</xml_diff>